<commit_message>
almost ready for second feedback
</commit_message>
<xml_diff>
--- a/Product Master Data.xlsx
+++ b/Product Master Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bff73b0ba30a6b9/Dokumen/College Files/OR/OR8/OR8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{50609603-6BD9-431A-B364-91EB3BAC3AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F4D9976-920B-4AAE-AF93-887CA188FB17}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="13_ncr:1_{50609603-6BD9-431A-B364-91EB3BAC3AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45DFD3D7-9937-4160-AE5E-DA5B25D543E8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="859" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="2810" windowWidth="14400" windowHeight="7270" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>SKU</t>
   </si>
@@ -48,12 +48,6 @@
     <t>COMM_NAME</t>
   </si>
   <si>
-    <t>WEIGHT_LBS_per_box</t>
-  </si>
-  <si>
-    <t>VOL_M3</t>
-  </si>
-  <si>
     <t>BOXES_PER_PALLET</t>
   </si>
   <si>
@@ -99,48 +93,18 @@
     <t>EU10202345</t>
   </si>
   <si>
-    <t>wireless skipping rope</t>
-  </si>
-  <si>
     <t>US12448263</t>
   </si>
   <si>
-    <t>chair fitness gym</t>
-  </si>
-  <si>
     <t>CH39932957</t>
   </si>
   <si>
-    <t>portable blender</t>
-  </si>
-  <si>
     <t>US77235921</t>
   </si>
   <si>
-    <t>underwater scooter</t>
-  </si>
-  <si>
     <t>CH88253013</t>
   </si>
   <si>
-    <t>aerial yoga swing</t>
-  </si>
-  <si>
-    <t>#DAYS (how many days of back up stock we need to have covered for the demand)</t>
-  </si>
-  <si>
-    <t>A product’s box typically contains one single item of that product.</t>
-  </si>
-  <si>
-    <t>Weight and volume is per box</t>
-  </si>
-  <si>
-    <t>The number of boxes per pallet always the same. But that doesn’t mean that the inbound capacity is the same as the</t>
-  </si>
-  <si>
-    <t>outbound capacity.</t>
-  </si>
-  <si>
     <t>FACTORY</t>
   </si>
   <si>
@@ -175,6 +139,12 @@
   </si>
   <si>
     <t>skiprope</t>
+  </si>
+  <si>
+    <t>WEIGHT_LBS_BOX</t>
+  </si>
+  <si>
+    <t>VOL_M3_BOX</t>
   </si>
 </sst>
 </file>
@@ -184,7 +154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -206,19 +176,13 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,12 +198,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -344,10 +302,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -358,16 +312,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -656,10 +609,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -690,60 +643,60 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="3">
         <v>1.0141199999999999</v>
@@ -799,18 +752,18 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="3">
         <v>5.0705999999999998</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="6">
         <v>9.7999999999999997E-3</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="7">
         <v>275</v>
       </c>
       <c r="F3">
@@ -858,10 +811,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="3">
         <v>1.02294</v>
@@ -917,10 +870,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="3">
         <v>6.7240900000000003</v>
@@ -976,10 +929,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="3">
         <v>7.3017000000000003</v>
@@ -1032,46 +985,6 @@
         <f>ROUNDUP(O6/H6,0)</f>
         <v>197</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K8" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1089,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BE37A0-A6EB-448C-9101-BEAA00E310D3}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1103,25 +1016,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="16" t="s">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>44</v>
+      <c r="A2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="5">
         <v>400</v>
@@ -1131,13 +1044,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="A3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="7">
         <v>275</v>
       </c>
       <c r="D3">
@@ -1145,11 +1058,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>41</v>
+      <c r="A4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="5">
         <v>336</v>
@@ -1159,11 +1072,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>42</v>
+      <c r="A5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="5">
         <v>120</v>
@@ -1173,11 +1086,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>43</v>
+      <c r="A6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="5">
         <v>480</v>
@@ -1201,7 +1114,7 @@
   <sheetData>
     <row r="1" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="4:4" x14ac:dyDescent="0.25">
@@ -1230,7 +1143,7 @@
       </c>
     </row>
     <row r="8" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D8" s="14"/>
+      <c r="D8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1248,7 +1161,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C1" t="b">
         <v>0</v>
@@ -1265,7 +1178,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -1301,21 +1214,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c024e8050b9bf00871c28df4e0c2326c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b87bd66fdc6a8cc420d7eafee76624a9" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -1530,24 +1428,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91E6C09D-371A-42AD-9131-71F13149D8CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC9CF9AD-F93B-4F3F-915C-4F16A1D231A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F75EFAFC-D66F-40E0-AF31-3A5730BD9E40}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1564,4 +1460,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC9CF9AD-F93B-4F3F-915C-4F16A1D231A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91E6C09D-371A-42AD-9131-71F13149D8CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>